<commit_message>
making wetness and temperature row-wise properties in the input table, removing global condtions and temp values from functions and tests
</commit_message>
<xml_diff>
--- a/tests/test_nds/v7.7-Deck-outercolumnline-ENVELOPE_test.xlsx
+++ b/tests/test_nds/v7.7-Deck-outercolumnline-ENVELOPE_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\SOMS\tests\test_nds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BF0966-B07D-4B5A-B62F-3F3ED239CCA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B98ED15-C5FE-49CA-89E7-BE1887EDE314}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="445">
   <si>
     <t xml:space="preserve">Ft' = </t>
   </si>
@@ -2890,6 +2890,15 @@
   </si>
   <si>
     <t>C_fire</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>100F&lt;T&lt;125F</t>
   </si>
 </sst>
 </file>
@@ -5166,10 +5175,10 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="78"/>
-    <col min="2" max="2" width="86.7265625" style="77" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="78"/>
+    <col min="2" max="2" width="86.7109375" style="77" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5182,7 +5191,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="30">
       <c r="A4" s="78">
         <v>1</v>
       </c>
@@ -5190,7 +5199,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="29">
+    <row r="5" spans="1:2" ht="30">
       <c r="A5" s="78">
         <v>2</v>
       </c>
@@ -5198,7 +5207,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="58">
+    <row r="6" spans="1:2" ht="75">
       <c r="A6" s="78">
         <v>3</v>
       </c>
@@ -5230,7 +5239,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="29">
+    <row r="10" spans="1:2" ht="30">
       <c r="A10" s="78">
         <v>7</v>
       </c>
@@ -5238,7 +5247,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="29">
+    <row r="11" spans="1:2" ht="30">
       <c r="A11" s="78">
         <v>8</v>
       </c>
@@ -5314,18 +5323,18 @@
       <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="10.1796875" customWidth="1"/>
-    <col min="5" max="5" width="4.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="9" width="5.7265625" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="9" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="15" width="5.7265625" customWidth="1"/>
-    <col min="16" max="16" width="7.54296875" customWidth="1"/>
-    <col min="17" max="17" width="9.54296875" customWidth="1"/>
-    <col min="18" max="18" width="7.54296875" customWidth="1"/>
+    <col min="12" max="15" width="5.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
+    <col min="18" max="18" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19">
@@ -5465,7 +5474,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="12" spans="2:19" ht="16.5">
+    <row r="12" spans="2:19" ht="18">
       <c r="D12" s="1" t="s">
         <v>99</v>
       </c>
@@ -5704,7 +5713,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="21" spans="2:33" ht="16.5">
+    <row r="21" spans="2:33" ht="18">
       <c r="D21" s="1" t="s">
         <v>87</v>
       </c>
@@ -5728,7 +5737,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="2:33" ht="16.5">
+    <row r="22" spans="2:33" ht="18">
       <c r="D22" s="1" t="s">
         <v>96</v>
       </c>
@@ -5779,7 +5788,7 @@
       <c r="G25" s="20"/>
       <c r="H25" s="9"/>
     </row>
-    <row r="26" spans="2:33" ht="15" thickBot="1">
+    <row r="26" spans="2:33" ht="15.75" thickBot="1">
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -6396,7 +6405,7 @@
         <v>1530000</v>
       </c>
     </row>
-    <row r="38" spans="2:26" ht="15" thickBot="1">
+    <row r="38" spans="2:26" ht="15.75" thickBot="1">
       <c r="B38" s="4" t="s">
         <v>5</v>
       </c>
@@ -6467,7 +6476,7 @@
       <c r="P39" s="35"/>
       <c r="Q39" s="35"/>
     </row>
-    <row r="40" spans="2:26" ht="15" thickBot="1">
+    <row r="40" spans="2:26" ht="15.75" thickBot="1">
       <c r="B40" s="8" t="s">
         <v>239</v>
       </c>
@@ -6494,7 +6503,7 @@
       </c>
       <c r="K41" s="38"/>
     </row>
-    <row r="42" spans="2:26" ht="17" thickBot="1">
+    <row r="42" spans="2:26" ht="18.75" thickBot="1">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="5" t="s">
@@ -6889,7 +6898,7 @@
         <v>2352.3150703451388</v>
       </c>
     </row>
-    <row r="54" spans="2:18" ht="15" thickBot="1">
+    <row r="54" spans="2:18" ht="15.75" thickBot="1">
       <c r="B54" s="4" t="s">
         <v>269</v>
       </c>
@@ -6923,7 +6932,7 @@
         <v>22536296.212499995</v>
       </c>
     </row>
-    <row r="55" spans="2:18" ht="16.5">
+    <row r="55" spans="2:18" ht="17.25">
       <c r="E55" s="53">
         <v>2</v>
       </c>
@@ -6931,7 +6940,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="56" spans="2:18" ht="16.5">
+    <row r="56" spans="2:18" ht="17.25">
       <c r="E56" s="53">
         <v>3</v>
       </c>
@@ -6939,7 +6948,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="2:18" ht="16.5">
+    <row r="59" spans="2:18" ht="18">
       <c r="B59" s="8" t="s">
         <v>33</v>
       </c>
@@ -7084,7 +7093,7 @@
     <row r="67" spans="2:18">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="2:18" ht="16.5">
+    <row r="68" spans="2:18" ht="18">
       <c r="B68" s="12" t="s">
         <v>42</v>
       </c>
@@ -7106,7 +7115,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="2:18" ht="16.5">
+    <row r="70" spans="2:18" ht="18">
       <c r="D70" s="1" t="s">
         <v>46</v>
       </c>
@@ -7121,7 +7130,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="2:18" ht="16.5">
+    <row r="71" spans="2:18" ht="18">
       <c r="D71" s="1" t="s">
         <v>46</v>
       </c>
@@ -7136,7 +7145,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="2:18" ht="16.5">
+    <row r="72" spans="2:18" ht="18">
       <c r="D72" s="1" t="s">
         <v>46</v>
       </c>
@@ -7151,7 +7160,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="2:18" ht="16.5">
+    <row r="73" spans="2:18" ht="18">
       <c r="D73" s="1" t="s">
         <v>46</v>
       </c>
@@ -7166,7 +7175,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="2:18" ht="16.5">
+    <row r="74" spans="2:18" ht="18">
       <c r="D74" s="1" t="s">
         <v>46</v>
       </c>
@@ -7181,7 +7190,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="2:18" ht="16.5">
+    <row r="75" spans="2:18" ht="18">
       <c r="D75" s="1" t="s">
         <v>46</v>
       </c>
@@ -7199,7 +7208,7 @@
     <row r="76" spans="2:18">
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="2:18" ht="16.5">
+    <row r="77" spans="2:18" ht="18">
       <c r="B77" s="8" t="s">
         <v>37</v>
       </c>
@@ -7225,7 +7234,7 @@
       <c r="N78" s="3"/>
       <c r="O78" s="55"/>
     </row>
-    <row r="79" spans="2:18" ht="16.5">
+    <row r="79" spans="2:18" ht="18">
       <c r="D79" s="1" t="s">
         <v>47</v>
       </c>
@@ -7240,7 +7249,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="2:18" ht="16.5">
+    <row r="80" spans="2:18" ht="18">
       <c r="D80" s="1" t="s">
         <v>47</v>
       </c>
@@ -7255,7 +7264,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="16.5">
+    <row r="82" spans="1:19" ht="18">
       <c r="A82" s="29"/>
       <c r="B82" s="8" t="s">
         <v>55</v>
@@ -7325,7 +7334,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="16.5">
+    <row r="85" spans="1:19" ht="18">
       <c r="D85" s="1" t="s">
         <v>333</v>
       </c>
@@ -7361,7 +7370,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="16.5">
+    <row r="86" spans="1:19" ht="18">
       <c r="D86" s="1" t="s">
         <v>334</v>
       </c>
@@ -7497,7 +7506,7 @@
         <v>22.985973359341013</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="16.5">
+    <row r="91" spans="1:19" ht="18">
       <c r="D91" s="1" t="s">
         <v>337</v>
       </c>
@@ -7519,7 +7528,7 @@
         <v>0.97750655522750263</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="16.5">
+    <row r="92" spans="1:19" ht="18">
       <c r="D92" s="1" t="s">
         <v>338</v>
       </c>
@@ -7545,7 +7554,7 @@
       <c r="D93" s="1"/>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:19" ht="16.5">
+    <row r="94" spans="1:19" ht="18">
       <c r="B94" s="8" t="s">
         <v>161</v>
       </c>
@@ -7616,7 +7625,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="16.5">
+    <row r="99" spans="1:11" ht="18">
       <c r="D99" s="113" t="s">
         <v>65</v>
       </c>
@@ -7628,7 +7637,7 @@
         <v>0.91110164655285553</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="16.5">
+    <row r="101" spans="1:11" ht="18">
       <c r="B101" s="8" t="s">
         <v>70</v>
       </c>
@@ -7654,7 +7663,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="16.5">
+    <row r="103" spans="1:11" ht="18">
       <c r="D103" s="1" t="s">
         <v>67</v>
       </c>
@@ -7666,7 +7675,7 @@
         <v>1.0390591181540647</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="16.5">
+    <row r="105" spans="1:11" ht="18">
       <c r="A105" s="1"/>
       <c r="B105" s="8" t="s">
         <v>71</v>
@@ -7729,7 +7738,7 @@
       </c>
       <c r="K108" s="133"/>
     </row>
-    <row r="109" spans="1:11" ht="16.5">
+    <row r="109" spans="1:11" ht="18">
       <c r="D109" s="1" t="s">
         <v>79</v>
       </c>
@@ -7741,7 +7750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="16.5">
+    <row r="111" spans="1:11" ht="18">
       <c r="A111" s="1"/>
       <c r="B111" s="8" t="s">
         <v>84</v>
@@ -7750,7 +7759,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="16.5">
+    <row r="112" spans="1:11" ht="18">
       <c r="D112" s="1" t="s">
         <v>76</v>
       </c>
@@ -7786,7 +7795,7 @@
       <c r="T114" s="45"/>
       <c r="U114" s="45"/>
     </row>
-    <row r="115" spans="1:21" ht="16.5">
+    <row r="115" spans="1:21" ht="18">
       <c r="D115" s="1" t="s">
         <v>83</v>
       </c>
@@ -7809,7 +7818,7 @@
       <c r="T115" s="45"/>
       <c r="U115" s="45"/>
     </row>
-    <row r="117" spans="1:21" ht="16.5">
+    <row r="117" spans="1:21" ht="18">
       <c r="B117" s="8" t="s">
         <v>85</v>
       </c>
@@ -8022,7 +8031,7 @@
         <v>0.60783335151037177</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="16.5">
+    <row r="125" spans="1:21" ht="18">
       <c r="D125" s="1" t="s">
         <v>108</v>
       </c>
@@ -8048,7 +8057,7 @@
       <c r="Q125" s="27"/>
       <c r="R125" s="27"/>
     </row>
-    <row r="127" spans="1:21" ht="16.5">
+    <row r="127" spans="1:21" ht="18">
       <c r="A127" s="1"/>
       <c r="B127" s="8" t="s">
         <v>109</v>
@@ -8057,7 +8066,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="16.5">
+    <row r="128" spans="1:21" ht="18">
       <c r="D128" s="1" t="s">
         <v>112</v>
       </c>
@@ -8162,7 +8171,7 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -8801,7 +8810,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -9107,16 +9116,16 @@
       <selection activeCell="V44" sqref="V44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
-    <col min="2" max="9" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="9" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="12" max="12" width="15.26953125" customWidth="1"/>
-    <col min="23" max="23" width="8.7265625" style="118"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="23" max="23" width="8.7109375" style="118"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1">
       <c r="B1" s="141" t="s">
         <v>127</v>
       </c>
@@ -9161,7 +9170,7 @@
       <c r="I2" s="150"/>
       <c r="R2" s="87"/>
     </row>
-    <row r="3" spans="1:18" ht="58">
+    <row r="3" spans="1:18" ht="60">
       <c r="A3" s="144"/>
       <c r="B3" s="146"/>
       <c r="C3" s="146"/>
@@ -9183,7 +9192,7 @@
       </c>
       <c r="R3" s="87"/>
     </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1">
       <c r="A4" s="144"/>
       <c r="B4" s="147"/>
       <c r="C4" s="147"/>
@@ -9206,7 +9215,7 @@
       <c r="J4" s="89"/>
       <c r="R4" s="87"/>
     </row>
-    <row r="5" spans="1:18" ht="15" thickBot="1">
+    <row r="5" spans="1:18" ht="15.75" thickBot="1">
       <c r="B5" s="108" t="s">
         <v>216</v>
       </c>
@@ -9469,7 +9478,7 @@
       </c>
       <c r="R16" s="87"/>
     </row>
-    <row r="17" spans="2:19" ht="15" thickBot="1">
+    <row r="17" spans="2:19" ht="15.75" thickBot="1">
       <c r="B17" s="138" t="s">
         <v>136</v>
       </c>
@@ -9597,7 +9606,7 @@
       </c>
       <c r="R23" s="87"/>
     </row>
-    <row r="24" spans="2:19" ht="16.5">
+    <row r="24" spans="2:19" ht="17.25">
       <c r="B24" s="88"/>
       <c r="C24" s="1" t="s">
         <v>117</v>
@@ -9628,7 +9637,7 @@
       </c>
       <c r="R24" s="87"/>
     </row>
-    <row r="25" spans="2:19" ht="16.5">
+    <row r="25" spans="2:19" ht="17.25">
       <c r="B25" s="88"/>
       <c r="C25" s="1" t="s">
         <v>118</v>
@@ -9659,7 +9668,7 @@
       </c>
       <c r="R25" s="87"/>
     </row>
-    <row r="26" spans="2:19" ht="16.5">
+    <row r="26" spans="2:19" ht="17.25">
       <c r="B26" s="88"/>
       <c r="C26" s="1" t="s">
         <v>119</v>
@@ -9721,7 +9730,7 @@
       </c>
       <c r="R27" s="87"/>
     </row>
-    <row r="28" spans="2:19" ht="16.5">
+    <row r="28" spans="2:19" ht="17.25">
       <c r="B28" s="89"/>
       <c r="C28" s="1" t="s">
         <v>121</v>
@@ -9752,7 +9761,7 @@
       </c>
       <c r="R28" s="87"/>
     </row>
-    <row r="29" spans="2:19" ht="16.5">
+    <row r="29" spans="2:19" ht="17.25">
       <c r="B29" s="89"/>
       <c r="C29" s="1" t="s">
         <v>122</v>
@@ -9835,7 +9844,7 @@
       </c>
       <c r="R32" s="87"/>
     </row>
-    <row r="33" spans="2:18" ht="16.5">
+    <row r="33" spans="2:18" ht="18">
       <c r="B33" s="100" t="s">
         <v>130</v>
       </c>
@@ -9872,7 +9881,7 @@
       </c>
       <c r="R33" s="87"/>
     </row>
-    <row r="34" spans="2:18" ht="17.5">
+    <row r="34" spans="2:18" ht="18.75">
       <c r="B34" s="100" t="s">
         <v>132</v>
       </c>
@@ -10655,7 +10664,7 @@
       </c>
       <c r="R62" s="87"/>
     </row>
-    <row r="63" spans="2:22" ht="16.5">
+    <row r="63" spans="2:22" ht="18">
       <c r="B63" s="100" t="s">
         <v>198</v>
       </c>
@@ -10969,7 +10978,7 @@
       <c r="N73" s="101"/>
       <c r="R73" s="87"/>
     </row>
-    <row r="74" spans="2:22" ht="15" thickBot="1">
+    <row r="74" spans="2:22" ht="15.75" thickBot="1">
       <c r="B74" s="105"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
@@ -11210,15 +11219,15 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="57" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" style="57" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" style="57" customWidth="1"/>
-    <col min="4" max="4" width="119.7265625" style="57" customWidth="1"/>
-    <col min="5" max="5" width="66.453125" style="57" customWidth="1"/>
-    <col min="6" max="23" width="9.1796875" style="57"/>
-    <col min="24" max="29" width="9.1796875" style="58"/>
+    <col min="1" max="1" width="8.7109375" style="57" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="57" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="57" customWidth="1"/>
+    <col min="4" max="4" width="119.7109375" style="57" customWidth="1"/>
+    <col min="5" max="5" width="66.42578125" style="57" customWidth="1"/>
+    <col min="6" max="23" width="9.140625" style="57"/>
+    <col min="24" max="29" width="9.140625" style="58"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">
@@ -11550,18 +11559,18 @@
   <dimension ref="A1:AJ13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" customWidth="1"/>
-    <col min="3" max="16" width="7.7265625" customWidth="1"/>
-    <col min="17" max="17" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="16" width="7.7109375" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="73" customHeight="1">
+    <row r="1" spans="1:36" ht="72.95" customHeight="1">
       <c r="A1" s="123" t="s">
         <v>379</v>
       </c>
@@ -11717,6 +11726,12 @@
       </c>
       <c r="Z2" s="127" t="s">
         <v>419</v>
+      </c>
+      <c r="AA2" s="127" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB2" s="127" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -11868,6 +11883,12 @@
       <c r="Z4">
         <v>900000</v>
       </c>
+      <c r="AA4" t="s">
+        <v>359</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="5" spans="1:36">
       <c r="B5" s="132"/>

</xml_diff>

<commit_message>
updating fire checks, test not passing yet
</commit_message>
<xml_diff>
--- a/tests/test_nds/v7.7-Deck-outercolumnline-ENVELOPE_test.xlsx
+++ b/tests/test_nds/v7.7-Deck-outercolumnline-ENVELOPE_test.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\SOMS\tests\test_nds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B98ED15-C5FE-49CA-89E7-BE1887EDE314}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5563A6BB-51AE-42A3-92E5-6D84D042FDF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="1170" windowWidth="28770" windowHeight="16170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
     <sheet name="Design Values" sheetId="1" r:id="rId2"/>
     <sheet name="Table" sheetId="8" r:id="rId3"/>
-    <sheet name="Fire" sheetId="9" r:id="rId4"/>
-    <sheet name="Member Checks" sheetId="4" r:id="rId5"/>
-    <sheet name="jb comments" sheetId="6" r:id="rId6"/>
-    <sheet name="Section Properties" sheetId="7" r:id="rId7"/>
+    <sheet name="Member Checks" sheetId="4" r:id="rId4"/>
+    <sheet name="DCR" sheetId="11" r:id="rId5"/>
+    <sheet name="Fire" sheetId="9" r:id="rId6"/>
+    <sheet name="DCR_Fire" sheetId="10" r:id="rId7"/>
+    <sheet name="jb comments" sheetId="6" r:id="rId8"/>
+    <sheet name="Section Properties" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Eminp">'Design Values'!$Q$38</definedName>
@@ -500,7 +502,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="464">
   <si>
     <t xml:space="preserve">Ft' = </t>
   </si>
@@ -2900,17 +2902,75 @@
   <si>
     <t>100F&lt;T&lt;125F</t>
   </si>
+  <si>
+    <t>Wetness condition</t>
+  </si>
+  <si>
+    <t>Service temperature</t>
+  </si>
+  <si>
+    <t>Effective char depth</t>
+  </si>
+  <si>
+    <t>Number of exposed sides</t>
+  </si>
+  <si>
+    <t>a_char</t>
+  </si>
+  <si>
+    <t>exp_b</t>
+  </si>
+  <si>
+    <t>exp_d</t>
+  </si>
+  <si>
+    <t>DCR_C</t>
+  </si>
+  <si>
+    <t>DCR_M3</t>
+  </si>
+  <si>
+    <t>DCR_M2</t>
+  </si>
+  <si>
+    <t>DCR_T</t>
+  </si>
+  <si>
+    <t>DCR_V</t>
+  </si>
+  <si>
+    <t>DCR_TM</t>
+  </si>
+  <si>
+    <t>DCR_CM</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#\ ???/???"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
     <numFmt numFmtId="168" formatCode="0.0E+00"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -3097,7 +3157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3167,6 +3227,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3539,7 +3617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3853,6 +3931,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4529,7 +4621,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>406585</xdr:colOff>
+      <xdr:colOff>406584</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>161983</xdr:rowOff>
     </xdr:to>
@@ -4617,7 +4709,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>181871</xdr:colOff>
+      <xdr:colOff>181872</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>50798</xdr:rowOff>
     </xdr:to>
@@ -4661,7 +4753,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>202487</xdr:colOff>
+      <xdr:colOff>202488</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
@@ -5319,8 +5411,8 @@
   </sheetPr>
   <dimension ref="A1:AG128"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P87" sqref="P87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5330,7 +5422,7 @@
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="9" width="5.7109375" customWidth="1"/>
     <col min="10" max="10" width="7.85546875" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="5.7109375" customWidth="1"/>
     <col min="16" max="16" width="7.5703125" customWidth="1"/>
     <col min="17" max="17" width="9.5703125" customWidth="1"/>
@@ -6226,16 +6318,16 @@
         <f>$D34*$F34*$G34*$H34</f>
         <v>81</v>
       </c>
-      <c r="T34" s="137" t="s">
+      <c r="T34" s="145" t="s">
         <v>163</v>
       </c>
-      <c r="U34" s="137"/>
-      <c r="V34" s="137"/>
-      <c r="X34" s="137" t="s">
+      <c r="U34" s="145"/>
+      <c r="V34" s="145"/>
+      <c r="X34" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="Y34" s="137"/>
-      <c r="Z34" s="137"/>
+      <c r="Y34" s="145"/>
+      <c r="Z34" s="145"/>
     </row>
     <row r="35" spans="2:26">
       <c r="B35" s="1" t="s">
@@ -6291,12 +6383,12 @@
         <f>$D35*$F35*$G35*$H35*$O35</f>
         <v>944.63503754238548</v>
       </c>
-      <c r="T35" s="137"/>
-      <c r="U35" s="137"/>
-      <c r="V35" s="137"/>
-      <c r="X35" s="137"/>
-      <c r="Y35" s="137"/>
-      <c r="Z35" s="137"/>
+      <c r="T35" s="145"/>
+      <c r="U35" s="145"/>
+      <c r="V35" s="145"/>
+      <c r="X35" s="145"/>
+      <c r="Y35" s="145"/>
+      <c r="Z35" s="145"/>
     </row>
     <row r="36" spans="2:26">
       <c r="B36" s="1" t="s">
@@ -6624,8 +6716,8 @@
       </c>
       <c r="I45" s="10"/>
       <c r="J45" s="51"/>
-      <c r="K45" s="28">
-        <f t="shared" ref="K45:K50" si="0">$D45*$F45</f>
+      <c r="K45" s="138">
+        <f>$D45*$F45</f>
         <v>31401.535253075766</v>
       </c>
     </row>
@@ -6655,7 +6747,7 @@
       <c r="I46" s="10"/>
       <c r="J46" s="18"/>
       <c r="K46" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K46:K49" si="0">$D46*$F46</f>
         <v>192828.75586217776</v>
       </c>
     </row>
@@ -6791,7 +6883,7 @@
         <v>32</v>
       </c>
       <c r="K50" s="28">
-        <f t="shared" si="0"/>
+        <f>$D50*$F50</f>
         <v>285</v>
       </c>
     </row>
@@ -6893,7 +6985,7 @@
       <c r="J53" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K53" s="28">
+      <c r="K53" s="139">
         <f>$D53*$F53</f>
         <v>2352.3150703451388</v>
       </c>
@@ -6969,18 +7061,18 @@
       <c r="G60" s="48" t="s">
         <v>226</v>
       </c>
-      <c r="I60" s="135" t="s">
+      <c r="I60" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="J60" s="135"/>
-      <c r="K60" s="135"/>
-      <c r="L60" s="135"/>
-      <c r="M60" s="135"/>
-      <c r="N60" s="135"/>
-      <c r="O60" s="135"/>
-      <c r="P60" s="135"/>
-      <c r="Q60" s="135"/>
-      <c r="R60" s="135"/>
+      <c r="J60" s="143"/>
+      <c r="K60" s="143"/>
+      <c r="L60" s="143"/>
+      <c r="M60" s="143"/>
+      <c r="N60" s="143"/>
+      <c r="O60" s="143"/>
+      <c r="P60" s="143"/>
+      <c r="Q60" s="143"/>
+      <c r="R60" s="143"/>
     </row>
     <row r="61" spans="2:18" ht="15" customHeight="1">
       <c r="D61" s="1" t="s">
@@ -6992,16 +7084,16 @@
       <c r="G61" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="I61" s="135"/>
-      <c r="J61" s="135"/>
-      <c r="K61" s="135"/>
-      <c r="L61" s="135"/>
-      <c r="M61" s="135"/>
-      <c r="N61" s="135"/>
-      <c r="O61" s="135"/>
-      <c r="P61" s="135"/>
-      <c r="Q61" s="135"/>
-      <c r="R61" s="135"/>
+      <c r="I61" s="143"/>
+      <c r="J61" s="143"/>
+      <c r="K61" s="143"/>
+      <c r="L61" s="143"/>
+      <c r="M61" s="143"/>
+      <c r="N61" s="143"/>
+      <c r="O61" s="143"/>
+      <c r="P61" s="143"/>
+      <c r="Q61" s="143"/>
+      <c r="R61" s="143"/>
     </row>
     <row r="62" spans="2:18">
       <c r="D62" s="1" t="s">
@@ -7013,16 +7105,16 @@
       <c r="G62" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="I62" s="135"/>
-      <c r="J62" s="135"/>
-      <c r="K62" s="135"/>
-      <c r="L62" s="135"/>
-      <c r="M62" s="135"/>
-      <c r="N62" s="135"/>
-      <c r="O62" s="135"/>
-      <c r="P62" s="135"/>
-      <c r="Q62" s="135"/>
-      <c r="R62" s="135"/>
+      <c r="I62" s="143"/>
+      <c r="J62" s="143"/>
+      <c r="K62" s="143"/>
+      <c r="L62" s="143"/>
+      <c r="M62" s="143"/>
+      <c r="N62" s="143"/>
+      <c r="O62" s="143"/>
+      <c r="P62" s="143"/>
+      <c r="Q62" s="143"/>
+      <c r="R62" s="143"/>
     </row>
     <row r="63" spans="2:18">
       <c r="D63" s="1" t="s">
@@ -7034,16 +7126,16 @@
       <c r="G63" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="I63" s="135"/>
-      <c r="J63" s="135"/>
-      <c r="K63" s="135"/>
-      <c r="L63" s="135"/>
-      <c r="M63" s="135"/>
-      <c r="N63" s="135"/>
-      <c r="O63" s="135"/>
-      <c r="P63" s="135"/>
-      <c r="Q63" s="135"/>
-      <c r="R63" s="135"/>
+      <c r="I63" s="143"/>
+      <c r="J63" s="143"/>
+      <c r="K63" s="143"/>
+      <c r="L63" s="143"/>
+      <c r="M63" s="143"/>
+      <c r="N63" s="143"/>
+      <c r="O63" s="143"/>
+      <c r="P63" s="143"/>
+      <c r="Q63" s="143"/>
+      <c r="R63" s="143"/>
     </row>
     <row r="64" spans="2:18">
       <c r="D64" s="1" t="s">
@@ -7055,16 +7147,16 @@
       <c r="G64" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="I64" s="135"/>
-      <c r="J64" s="135"/>
-      <c r="K64" s="135"/>
-      <c r="L64" s="135"/>
-      <c r="M64" s="135"/>
-      <c r="N64" s="135"/>
-      <c r="O64" s="135"/>
-      <c r="P64" s="135"/>
-      <c r="Q64" s="135"/>
-      <c r="R64" s="135"/>
+      <c r="I64" s="143"/>
+      <c r="J64" s="143"/>
+      <c r="K64" s="143"/>
+      <c r="L64" s="143"/>
+      <c r="M64" s="143"/>
+      <c r="N64" s="143"/>
+      <c r="O64" s="143"/>
+      <c r="P64" s="143"/>
+      <c r="Q64" s="143"/>
+      <c r="R64" s="143"/>
     </row>
     <row r="65" spans="2:18">
       <c r="D65" s="1" t="s">
@@ -7076,16 +7168,16 @@
       <c r="G65" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="I65" s="135"/>
-      <c r="J65" s="135"/>
-      <c r="K65" s="135"/>
-      <c r="L65" s="135"/>
-      <c r="M65" s="135"/>
-      <c r="N65" s="135"/>
-      <c r="O65" s="135"/>
-      <c r="P65" s="135"/>
-      <c r="Q65" s="135"/>
-      <c r="R65" s="135"/>
+      <c r="I65" s="143"/>
+      <c r="J65" s="143"/>
+      <c r="K65" s="143"/>
+      <c r="L65" s="143"/>
+      <c r="M65" s="143"/>
+      <c r="N65" s="143"/>
+      <c r="O65" s="143"/>
+      <c r="P65" s="143"/>
+      <c r="Q65" s="143"/>
+      <c r="R65" s="143"/>
     </row>
     <row r="66" spans="2:18">
       <c r="L66" s="1"/>
@@ -7226,10 +7318,10 @@
       <c r="E78" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F78" s="136" t="s">
+      <c r="F78" s="144" t="s">
         <v>88</v>
       </c>
-      <c r="G78" s="136"/>
+      <c r="G78" s="144"/>
       <c r="M78" s="1"/>
       <c r="N78" s="3"/>
       <c r="O78" s="55"/>
@@ -7724,19 +7816,19 @@
       <c r="E108" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F108" s="134" t="str">
+      <c r="F108" s="142" t="str">
         <f>IF($F$107=0, "N/A", $F$106/$F$107)</f>
         <v>N/A</v>
       </c>
-      <c r="G108" s="134"/>
+      <c r="G108" s="142"/>
       <c r="H108" t="s">
         <v>75</v>
       </c>
-      <c r="J108" s="133">
+      <c r="J108" s="141">
         <f>IF(OR(F3="Southern Pine",F3="Hardwood"),1/100,1/125)</f>
         <v>0.01</v>
       </c>
-      <c r="K108" s="133"/>
+      <c r="K108" s="141"/>
     </row>
     <row r="109" spans="1:11" ht="18">
       <c r="D109" s="1" t="s">
@@ -8168,7 +8260,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8803,317 +8895,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5619B72B-1023-4122-B29E-C718AB977089}">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1" t="s">
-        <v>441</v>
-      </c>
-      <c r="C1" t="s">
-        <v>435</v>
-      </c>
-      <c r="D1" t="s">
-        <v>436</v>
-      </c>
-      <c r="E1" t="s">
-        <v>437</v>
-      </c>
-      <c r="F1" t="s">
-        <v>438</v>
-      </c>
-      <c r="G1" t="s">
-        <v>425</v>
-      </c>
-      <c r="H1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>439</v>
-      </c>
-      <c r="B2">
-        <f>'Design Values'!F43</f>
-        <v>2.85</v>
-      </c>
-      <c r="C2">
-        <f>'Design Values'!G43</f>
-        <v>0.91110164655285553</v>
-      </c>
-      <c r="D2" t="str">
-        <f>'Design Values'!H43</f>
-        <v>-</v>
-      </c>
-      <c r="E2">
-        <f>'Design Values'!I43</f>
-        <v>0.97750655522750263</v>
-      </c>
-      <c r="F2" t="str">
-        <f>'Design Values'!J43</f>
-        <v>-</v>
-      </c>
-      <c r="G2">
-        <f>'Design Values'!D43</f>
-        <v>1750</v>
-      </c>
-      <c r="H2">
-        <f>'Design Values'!K43</f>
-        <v>4544.119462182367</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>429</v>
-      </c>
-      <c r="B3">
-        <f>'Design Values'!F44</f>
-        <v>2.85</v>
-      </c>
-      <c r="C3" t="str">
-        <f>'Design Values'!G44</f>
-        <v>-</v>
-      </c>
-      <c r="D3">
-        <f>'Design Values'!H44</f>
-        <v>1.0390591181540647</v>
-      </c>
-      <c r="E3">
-        <f>'Design Values'!I44</f>
-        <v>0.99773634010879775</v>
-      </c>
-      <c r="F3" t="str">
-        <f>'Design Values'!J44</f>
-        <v>-</v>
-      </c>
-      <c r="G3">
-        <f>'Design Values'!D44</f>
-        <v>1450</v>
-      </c>
-      <c r="H3">
-        <f>'Design Values'!K44</f>
-        <v>4284.1918498405876</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>430</v>
-      </c>
-      <c r="B4">
-        <f>'Design Values'!F47</f>
-        <v>2.85</v>
-      </c>
-      <c r="C4" t="str">
-        <f>'Design Values'!G47</f>
-        <v>-</v>
-      </c>
-      <c r="D4" t="str">
-        <f>'Design Values'!H47</f>
-        <v>-</v>
-      </c>
-      <c r="E4" t="str">
-        <f>'Design Values'!I47</f>
-        <v>-</v>
-      </c>
-      <c r="F4" t="str">
-        <f>'Design Values'!J47</f>
-        <v>-</v>
-      </c>
-      <c r="G4">
-        <f>'Design Values'!D47</f>
-        <v>1100</v>
-      </c>
-      <c r="H4">
-        <f>'Design Values'!K47</f>
-        <v>3135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>431</v>
-      </c>
-      <c r="B5">
-        <f>'Design Values'!F48</f>
-        <v>2.75</v>
-      </c>
-      <c r="C5" t="str">
-        <f>'Design Values'!G48</f>
-        <v>-</v>
-      </c>
-      <c r="D5" t="str">
-        <f>'Design Values'!H48</f>
-        <v>-</v>
-      </c>
-      <c r="E5" t="str">
-        <f>'Design Values'!I48</f>
-        <v>-</v>
-      </c>
-      <c r="F5" t="str">
-        <f>'Design Values'!J48</f>
-        <v>-</v>
-      </c>
-      <c r="G5">
-        <f>'Design Values'!D48</f>
-        <v>260</v>
-      </c>
-      <c r="H5">
-        <f>'Design Values'!K48</f>
-        <v>715</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>432</v>
-      </c>
-      <c r="B6">
-        <f>'Design Values'!F49</f>
-        <v>2.75</v>
-      </c>
-      <c r="C6" t="str">
-        <f>'Design Values'!G49</f>
-        <v>-</v>
-      </c>
-      <c r="D6" t="str">
-        <f>'Design Values'!H49</f>
-        <v>-</v>
-      </c>
-      <c r="E6" t="str">
-        <f>'Design Values'!I49</f>
-        <v>-</v>
-      </c>
-      <c r="F6" t="str">
-        <f>'Design Values'!J49</f>
-        <v>-</v>
-      </c>
-      <c r="G6">
-        <f>'Design Values'!D49</f>
-        <v>300</v>
-      </c>
-      <c r="H6">
-        <f>'Design Values'!K49</f>
-        <v>825</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>433</v>
-      </c>
-      <c r="B7">
-        <f>'Design Values'!F50</f>
-        <v>2.85</v>
-      </c>
-      <c r="C7" t="str">
-        <f>'Design Values'!G50</f>
-        <v>-</v>
-      </c>
-      <c r="D7" t="str">
-        <f>'Design Values'!H50</f>
-        <v>-</v>
-      </c>
-      <c r="E7" t="str">
-        <f>'Design Values'!I50</f>
-        <v>-</v>
-      </c>
-      <c r="F7" t="str">
-        <f>'Design Values'!J50</f>
-        <v>-</v>
-      </c>
-      <c r="G7">
-        <f>'Design Values'!D50</f>
-        <v>100</v>
-      </c>
-      <c r="H7">
-        <f>'Design Values'!K50</f>
-        <v>285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>434</v>
-      </c>
-      <c r="B8">
-        <f>'Design Values'!F51</f>
-        <v>2.58</v>
-      </c>
-      <c r="C8" t="str">
-        <f>'Design Values'!G51</f>
-        <v>-</v>
-      </c>
-      <c r="D8" t="str">
-        <f>'Design Values'!H51</f>
-        <v>-</v>
-      </c>
-      <c r="E8" t="str">
-        <f>'Design Values'!I51</f>
-        <v>-</v>
-      </c>
-      <c r="F8">
-        <f>'Design Values'!J51</f>
-        <v>0.5432283962107034</v>
-      </c>
-      <c r="G8">
-        <f>'Design Values'!D51</f>
-        <v>1500</v>
-      </c>
-      <c r="H8">
-        <f>'Design Values'!K51</f>
-        <v>2102.2938933354221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>440</v>
-      </c>
-      <c r="B9">
-        <f>'Design Values'!F52</f>
-        <v>2.58</v>
-      </c>
-      <c r="C9" t="str">
-        <f>'Design Values'!G52</f>
-        <v>-</v>
-      </c>
-      <c r="D9" t="str">
-        <f>'Design Values'!H52</f>
-        <v>-</v>
-      </c>
-      <c r="E9" t="str">
-        <f>'Design Values'!I52</f>
-        <v>-</v>
-      </c>
-      <c r="F9" t="str">
-        <f>'Design Values'!J52</f>
-        <v>-</v>
-      </c>
-      <c r="G9">
-        <f>'Design Values'!D52</f>
-        <v>650</v>
-      </c>
-      <c r="H9">
-        <f>'Design Values'!K52</f>
-        <v>1677</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V44" sqref="V44"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V65" sqref="V65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9122,20 +8909,22 @@
     <col min="2" max="9" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.7109375" style="118"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="149" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="143"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="151"/>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
       <c r="L1" s="35"/>
@@ -9147,34 +8936,34 @@
       <c r="R1" s="86"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="144"/>
-      <c r="B2" s="145" t="s">
+      <c r="A2" s="152"/>
+      <c r="B2" s="153" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="145" t="s">
+      <c r="C2" s="153" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="151" t="s">
+      <c r="D2" s="159" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="148" t="s">
+      <c r="F2" s="156" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="149"/>
-      <c r="H2" s="148" t="s">
+      <c r="G2" s="157"/>
+      <c r="H2" s="156" t="s">
         <v>153</v>
       </c>
-      <c r="I2" s="150"/>
+      <c r="I2" s="158"/>
       <c r="R2" s="87"/>
     </row>
     <row r="3" spans="1:18" ht="60">
-      <c r="A3" s="144"/>
-      <c r="B3" s="146"/>
-      <c r="C3" s="146"/>
-      <c r="D3" s="152"/>
+      <c r="A3" s="152"/>
+      <c r="B3" s="154"/>
+      <c r="C3" s="154"/>
+      <c r="D3" s="160"/>
       <c r="E3" s="63" t="s">
         <v>349</v>
       </c>
@@ -9193,10 +8982,10 @@
       <c r="R3" s="87"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A4" s="144"/>
-      <c r="B4" s="147"/>
-      <c r="C4" s="147"/>
-      <c r="D4" s="153"/>
+      <c r="A4" s="152"/>
+      <c r="B4" s="155"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="161"/>
       <c r="E4" s="32" t="s">
         <v>114</v>
       </c>
@@ -9479,25 +9268,25 @@
       <c r="R16" s="87"/>
     </row>
     <row r="17" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B17" s="138" t="s">
+      <c r="B17" s="146" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="139"/>
-      <c r="D17" s="139"/>
-      <c r="E17" s="139"/>
-      <c r="F17" s="139"/>
-      <c r="G17" s="139"/>
-      <c r="H17" s="139"/>
-      <c r="I17" s="139"/>
-      <c r="J17" s="139"/>
-      <c r="K17" s="139"/>
-      <c r="L17" s="139"/>
-      <c r="M17" s="139"/>
-      <c r="N17" s="139"/>
-      <c r="O17" s="139"/>
-      <c r="P17" s="139"/>
-      <c r="Q17" s="139"/>
-      <c r="R17" s="140"/>
+      <c r="C17" s="147"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="147"/>
+      <c r="F17" s="147"/>
+      <c r="G17" s="147"/>
+      <c r="H17" s="147"/>
+      <c r="I17" s="147"/>
+      <c r="J17" s="147"/>
+      <c r="K17" s="147"/>
+      <c r="L17" s="147"/>
+      <c r="M17" s="147"/>
+      <c r="N17" s="147"/>
+      <c r="O17" s="147"/>
+      <c r="P17" s="147"/>
+      <c r="Q17" s="147"/>
+      <c r="R17" s="148"/>
       <c r="S17" s="8"/>
     </row>
     <row r="18" spans="2:19">
@@ -10658,7 +10447,7 @@
       <c r="N62" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="O62" s="26">
+      <c r="O62" s="137">
         <f>K61/O58</f>
         <v>1.6424529378451411E-5</v>
       </c>
@@ -10892,7 +10681,7 @@
       <c r="J69" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="K69" s="93">
+      <c r="K69" s="140">
         <f>1-K61/O58-(K65/K64)^2</f>
         <v>0.97728856713306311</v>
       </c>
@@ -10925,7 +10714,7 @@
       <c r="J70" s="117" t="s">
         <v>187</v>
       </c>
-      <c r="K70" s="26">
+      <c r="K70" s="136">
         <f>(K61/Fcf)^2+K65/(O68*K68)+O65/(O69*K69)</f>
         <v>0.74491816422522406</v>
       </c>
@@ -11208,7 +10997,518 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70002DF1-385F-4EB3-93AE-AEA121A3E10F}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1" t="s">
+        <v>463</v>
+      </c>
+      <c r="F1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G1" t="s">
+        <v>454</v>
+      </c>
+      <c r="H1" t="s">
+        <v>452</v>
+      </c>
+      <c r="I1" t="s">
+        <v>455</v>
+      </c>
+      <c r="J1" t="s">
+        <v>456</v>
+      </c>
+      <c r="K1" t="s">
+        <v>457</v>
+      </c>
+      <c r="L1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <f>'Member Checks'!E5</f>
+        <v>-37</v>
+      </c>
+      <c r="B2">
+        <f>'Member Checks'!F5</f>
+        <v>66</v>
+      </c>
+      <c r="C2">
+        <f>'Member Checks'!G5</f>
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <f>'Member Checks'!H5</f>
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <f>'Member Checks'!I5</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="26">
+        <f>'Member Checks'!G35</f>
+        <v>0.84546891794538326</v>
+      </c>
+      <c r="G2" s="26">
+        <f>'Member Checks'!G40</f>
+        <v>0.11491239472353589</v>
+      </c>
+      <c r="H2" s="26">
+        <f>'Member Checks'!C40</f>
+        <v>0.1920027754755706</v>
+      </c>
+      <c r="I2" s="26">
+        <f>'Member Checks'!C45</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="26">
+        <f>'Member Checks'!G45</f>
+        <v>0.27233115468409586</v>
+      </c>
+      <c r="K2" s="26">
+        <f>MAX('Member Checks'!G50,'Member Checks'!G52)</f>
+        <v>0.95891529456195657</v>
+      </c>
+      <c r="L2" s="26">
+        <f>MAX('Member Checks'!C70:C71)</f>
+        <v>1.1051180503497853</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5619B72B-1023-4122-B29E-C718AB977089}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F1" t="s">
+        <v>438</v>
+      </c>
+      <c r="G1" t="s">
+        <v>425</v>
+      </c>
+      <c r="H1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B2">
+        <f>'Design Values'!F43</f>
+        <v>2.85</v>
+      </c>
+      <c r="C2">
+        <f>'Design Values'!G43</f>
+        <v>0.91110164655285553</v>
+      </c>
+      <c r="D2" t="str">
+        <f>'Design Values'!H43</f>
+        <v>-</v>
+      </c>
+      <c r="E2">
+        <f>'Design Values'!I43</f>
+        <v>0.97750655522750263</v>
+      </c>
+      <c r="F2" t="str">
+        <f>'Design Values'!J43</f>
+        <v>-</v>
+      </c>
+      <c r="G2">
+        <f>'Design Values'!D43</f>
+        <v>1750</v>
+      </c>
+      <c r="H2">
+        <f>'Design Values'!K43</f>
+        <v>4544.119462182367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B3">
+        <f>'Design Values'!F44</f>
+        <v>2.85</v>
+      </c>
+      <c r="C3" t="str">
+        <f>'Design Values'!G44</f>
+        <v>-</v>
+      </c>
+      <c r="D3">
+        <f>'Design Values'!H44</f>
+        <v>1.0390591181540647</v>
+      </c>
+      <c r="E3">
+        <f>'Design Values'!I44</f>
+        <v>0.99773634010879775</v>
+      </c>
+      <c r="F3" t="str">
+        <f>'Design Values'!J44</f>
+        <v>-</v>
+      </c>
+      <c r="G3">
+        <f>'Design Values'!D44</f>
+        <v>1450</v>
+      </c>
+      <c r="H3">
+        <f>'Design Values'!K44</f>
+        <v>4284.1918498405876</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B4">
+        <f>'Design Values'!F47</f>
+        <v>2.85</v>
+      </c>
+      <c r="C4" t="str">
+        <f>'Design Values'!G47</f>
+        <v>-</v>
+      </c>
+      <c r="D4" t="str">
+        <f>'Design Values'!H47</f>
+        <v>-</v>
+      </c>
+      <c r="E4" t="str">
+        <f>'Design Values'!I47</f>
+        <v>-</v>
+      </c>
+      <c r="F4" t="str">
+        <f>'Design Values'!J47</f>
+        <v>-</v>
+      </c>
+      <c r="G4">
+        <f>'Design Values'!D47</f>
+        <v>1100</v>
+      </c>
+      <c r="H4">
+        <f>'Design Values'!K47</f>
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>431</v>
+      </c>
+      <c r="B5">
+        <f>'Design Values'!F48</f>
+        <v>2.75</v>
+      </c>
+      <c r="C5" t="str">
+        <f>'Design Values'!G48</f>
+        <v>-</v>
+      </c>
+      <c r="D5" t="str">
+        <f>'Design Values'!H48</f>
+        <v>-</v>
+      </c>
+      <c r="E5" t="str">
+        <f>'Design Values'!I48</f>
+        <v>-</v>
+      </c>
+      <c r="F5" t="str">
+        <f>'Design Values'!J48</f>
+        <v>-</v>
+      </c>
+      <c r="G5">
+        <f>'Design Values'!D48</f>
+        <v>260</v>
+      </c>
+      <c r="H5">
+        <f>'Design Values'!K48</f>
+        <v>715</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>432</v>
+      </c>
+      <c r="B6">
+        <f>'Design Values'!F49</f>
+        <v>2.75</v>
+      </c>
+      <c r="C6" t="str">
+        <f>'Design Values'!G49</f>
+        <v>-</v>
+      </c>
+      <c r="D6" t="str">
+        <f>'Design Values'!H49</f>
+        <v>-</v>
+      </c>
+      <c r="E6" t="str">
+        <f>'Design Values'!I49</f>
+        <v>-</v>
+      </c>
+      <c r="F6" t="str">
+        <f>'Design Values'!J49</f>
+        <v>-</v>
+      </c>
+      <c r="G6">
+        <f>'Design Values'!D49</f>
+        <v>300</v>
+      </c>
+      <c r="H6">
+        <f>'Design Values'!K49</f>
+        <v>825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>433</v>
+      </c>
+      <c r="B7">
+        <f>'Design Values'!F50</f>
+        <v>2.85</v>
+      </c>
+      <c r="C7" t="str">
+        <f>'Design Values'!G50</f>
+        <v>-</v>
+      </c>
+      <c r="D7" t="str">
+        <f>'Design Values'!H50</f>
+        <v>-</v>
+      </c>
+      <c r="E7" t="str">
+        <f>'Design Values'!I50</f>
+        <v>-</v>
+      </c>
+      <c r="F7" t="str">
+        <f>'Design Values'!J50</f>
+        <v>-</v>
+      </c>
+      <c r="G7">
+        <f>'Design Values'!D50</f>
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <f>'Design Values'!K50</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>434</v>
+      </c>
+      <c r="B8">
+        <f>'Design Values'!F51</f>
+        <v>2.58</v>
+      </c>
+      <c r="C8" t="str">
+        <f>'Design Values'!G51</f>
+        <v>-</v>
+      </c>
+      <c r="D8" t="str">
+        <f>'Design Values'!H51</f>
+        <v>-</v>
+      </c>
+      <c r="E8" t="str">
+        <f>'Design Values'!I51</f>
+        <v>-</v>
+      </c>
+      <c r="F8">
+        <f>'Design Values'!J51</f>
+        <v>0.5432283962107034</v>
+      </c>
+      <c r="G8">
+        <f>'Design Values'!D51</f>
+        <v>1500</v>
+      </c>
+      <c r="H8">
+        <f>'Design Values'!K51</f>
+        <v>2102.2938933354221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>440</v>
+      </c>
+      <c r="B9">
+        <f>'Design Values'!F52</f>
+        <v>2.58</v>
+      </c>
+      <c r="C9" t="str">
+        <f>'Design Values'!G52</f>
+        <v>-</v>
+      </c>
+      <c r="D9" t="str">
+        <f>'Design Values'!H52</f>
+        <v>-</v>
+      </c>
+      <c r="E9" t="str">
+        <f>'Design Values'!I52</f>
+        <v>-</v>
+      </c>
+      <c r="F9" t="str">
+        <f>'Design Values'!J52</f>
+        <v>-</v>
+      </c>
+      <c r="G9">
+        <f>'Design Values'!D52</f>
+        <v>650</v>
+      </c>
+      <c r="H9">
+        <f>'Design Values'!K52</f>
+        <v>1677</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B1ADAB-A93D-475E-944B-53925D047810}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1" t="s">
+        <v>463</v>
+      </c>
+      <c r="F1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G1" t="s">
+        <v>454</v>
+      </c>
+      <c r="H1" t="s">
+        <v>452</v>
+      </c>
+      <c r="I1" t="s">
+        <v>455</v>
+      </c>
+      <c r="J1" t="s">
+        <v>456</v>
+      </c>
+      <c r="K1" t="s">
+        <v>457</v>
+      </c>
+      <c r="L1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <f>'Member Checks'!E5</f>
+        <v>-37</v>
+      </c>
+      <c r="B2">
+        <f>'Member Checks'!F5</f>
+        <v>66</v>
+      </c>
+      <c r="C2">
+        <f>'Member Checks'!G5</f>
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <f>'Member Checks'!H5</f>
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <f>'Member Checks'!I5</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="26">
+        <f>'Member Checks'!O35</f>
+        <v>0.51282628497350602</v>
+      </c>
+      <c r="G2" s="26">
+        <f>'Member Checks'!O40</f>
+        <v>0.10293486824976555</v>
+      </c>
+      <c r="H2" s="26">
+        <f>'Member Checks'!K40</f>
+        <v>0.17606865548014611</v>
+      </c>
+      <c r="I2" s="26">
+        <f>'Member Checks'!K45</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="26">
+        <f>'Member Checks'!O45</f>
+        <v>0.14551275055476737</v>
+      </c>
+      <c r="K2" s="26">
+        <f>MAX('Member Checks'!O50,'Member Checks'!O52)</f>
+        <v>0.60399291397167176</v>
+      </c>
+      <c r="L2" s="26">
+        <f>MAX('Member Checks'!K70:K71)</f>
+        <v>0.74491816422522406</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFFC7CE"/>
@@ -11554,12 +11854,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA22655-602E-48EB-ABE9-4ED6FD40E209}">
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB14" sqref="AB14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11568,6 +11868,8 @@
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="16" width="7.7109375" customWidth="1"/>
     <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="72.95" customHeight="1">
@@ -11647,6 +11949,21 @@
       <c r="Z1" s="124" t="s">
         <v>403</v>
       </c>
+      <c r="AA1" s="124" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB1" s="124" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC1" s="124" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD1" s="124" t="s">
+        <v>448</v>
+      </c>
+      <c r="AE1" s="124" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="2" spans="1:36">
       <c r="A2" s="125" t="s">
@@ -11727,11 +12044,20 @@
       <c r="Z2" s="127" t="s">
         <v>419</v>
       </c>
-      <c r="AA2" s="127" t="s">
+      <c r="AA2" s="133" t="s">
         <v>442</v>
       </c>
-      <c r="AB2" s="127" t="s">
+      <c r="AB2" s="133" t="s">
         <v>443</v>
+      </c>
+      <c r="AC2" s="134" t="s">
+        <v>449</v>
+      </c>
+      <c r="AD2" s="134" t="s">
+        <v>450</v>
+      </c>
+      <c r="AE2" s="134" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -11803,6 +12129,11 @@
       <c r="Z3" s="130" t="s">
         <v>104</v>
       </c>
+      <c r="AC3" s="135" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD3" s="135"/>
+      <c r="AE3" s="135"/>
     </row>
     <row r="4" spans="1:36">
       <c r="A4" s="131" t="s">
@@ -11888,6 +12219,15 @@
       </c>
       <c r="AB4" t="s">
         <v>444</v>
+      </c>
+      <c r="AC4">
+        <v>1.8</v>
+      </c>
+      <c r="AD4">
+        <v>2</v>
+      </c>
+      <c r="AE4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:36">

</xml_diff>